<commit_message>
CI changes - Till pre-app dashboard page
</commit_message>
<xml_diff>
--- a/UAA/src/src/test/resources/com/ugapp/excel/testdata.xlsx
+++ b/UAA/src/src/test/resources/com/ugapp/excel/testdata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="112">
   <si>
     <t>TCID</t>
   </si>
@@ -348,6 +348,21 @@
   </si>
   <si>
     <t>July 19, 1926</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>699129@test.asu.edu</t>
+  </si>
+  <si>
+    <t>May 18, 1961</t>
+  </si>
+  <si>
+    <t>September 6, 1953</t>
   </si>
 </sst>
 </file>
@@ -435,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -458,6 +473,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
@@ -3119,7 +3152,12 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="B1" s="3"/>
+      <c r="A1" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>109</v>
+      </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
       <c r="F1" s="3"/>
@@ -3132,7 +3170,7 @@
       <c r="A2" t="s" s="0">
         <v>102</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="20" t="s">
         <v>103</v>
       </c>
       <c r="D2" s="3"/>
@@ -3146,7 +3184,7 @@
       <c r="A3" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="3"/>
@@ -3160,8 +3198,8 @@
       <c r="A4" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>106</v>
+      <c r="B4" s="22" t="s">
+        <v>111</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>

</xml_diff>

<commit_message>
Base code till Login page
</commit_message>
<xml_diff>
--- a/UAA/src/src/test/resources/com/ugapp/excel/testdata.xlsx
+++ b/UAA/src/src/test/resources/com/ugapp/excel/testdata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="104">
   <si>
     <t>TCID</t>
   </si>
@@ -335,34 +335,10 @@
     <t>Test Degree</t>
   </si>
   <si>
-    <t>Legal name</t>
-  </si>
-  <si>
-    <t>Test FN Automation MN Test LN</t>
-  </si>
-  <si>
-    <t>Preferred first name</t>
-  </si>
-  <si>
-    <t>Date of birth</t>
-  </si>
-  <si>
-    <t>July 19, 1926</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>699129@test.asu.edu</t>
-  </si>
-  <si>
-    <t>May 18, 1961</t>
-  </si>
-  <si>
-    <t>September 6, 1953</t>
+    <t>164313@test.asu.edu</t>
   </si>
 </sst>
 </file>
@@ -450,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -473,30 +449,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
@@ -3153,10 +3105,10 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="0">
-        <v>107</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>109</v>
+        <v>102</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
@@ -3167,12 +3119,8 @@
       <c r="L1" s="3"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="0">
-        <v>102</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>103</v>
-      </c>
+      <c r="A2" s="4"/>
+      <c r="B2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="3"/>
@@ -3181,12 +3129,8 @@
       <c r="L2" s="3"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="0">
-        <v>104</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>29</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
       <c r="F3" s="3"/>
@@ -3195,12 +3139,8 @@
       <c r="L3" s="3"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="0">
-        <v>105</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>111</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
       <c r="F4" s="3"/>

</xml_diff>

<commit_message>
Base code till My information for F1_Greater24_US_Res_SpouseDependent_FutureGrad_InstateSchool_OOS_ABOR
</commit_message>
<xml_diff>
--- a/UAA/src/src/test/resources/com/ugapp/excel/testdata.xlsx
+++ b/UAA/src/src/test/resources/com/ugapp/excel/testdata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="162">
   <si>
     <t>TCID</t>
   </si>
@@ -339,6 +339,204 @@
   </si>
   <si>
     <t>164313@test.asu.edu</t>
+  </si>
+  <si>
+    <t>539397@test.asu.edu</t>
+  </si>
+  <si>
+    <t>512665@test.asu.edu</t>
+  </si>
+  <si>
+    <t>345148@test.asu.edu</t>
+  </si>
+  <si>
+    <t>Legal name</t>
+  </si>
+  <si>
+    <t>Test FN Automation MN Test LN</t>
+  </si>
+  <si>
+    <t>Preferred first name</t>
+  </si>
+  <si>
+    <t>Date of birth</t>
+  </si>
+  <si>
+    <t>January 21, 1968</t>
+  </si>
+  <si>
+    <t>Legal sex</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Primary language spoken at home</t>
+  </si>
+  <si>
+    <t>German, Swiss</t>
+  </si>
+  <si>
+    <t>Home address</t>
+  </si>
+  <si>
+    <t>Test Address line1 Test Address line2
+TestTestTestTestTestTestTestTest,Tavus,Armenia
+12345-678910</t>
+  </si>
+  <si>
+    <t>Test Address line1 Test Address line2
+Test City,Ararat,Armenia
+12345-678910</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethnic/racial background </t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>U.S. citizenship</t>
+  </si>
+  <si>
+    <t>I am a U.S. citizen</t>
+  </si>
+  <si>
+    <t>Country of citizenship</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Country of birth</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Social Security Number</t>
+  </si>
+  <si>
+    <t>*********</t>
+  </si>
+  <si>
+    <t>Parent or legal guardian</t>
+  </si>
+  <si>
+    <t>Parent FN Parent LN I</t>
+  </si>
+  <si>
+    <t>Parent or Legal Guardian Relation</t>
+  </si>
+  <si>
+    <t>Mother</t>
+  </si>
+  <si>
+    <t>Parent or Legal Guardian Schooling Level</t>
+  </si>
+  <si>
+    <t>College or Beyond</t>
+  </si>
+  <si>
+    <t>Additional parent or legal guardian</t>
+  </si>
+  <si>
+    <t>Parent FN Parent LN II</t>
+  </si>
+  <si>
+    <t>Sibling</t>
+  </si>
+  <si>
+    <t>Other/Unknown</t>
+  </si>
+  <si>
+    <t>Previous ASU affiliation</t>
+  </si>
+  <si>
+    <t>I have never been affiliated with Arizona State University</t>
+  </si>
+  <si>
+    <t>Military status</t>
+  </si>
+  <si>
+    <t>I am the spouse/dependent of a U.S. service member or veteran</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>United States Space Force
+United States Army
+United States Marine Corps
+United States Navy
+United States Air Force
+United States Coast Guard
+United States Space Force
+United States Public Health Service Commissioned Corps
+National Oceanic and Atmospheric Administration Commissioned Officer Corps</t>
+  </si>
+  <si>
+    <t>I have applied or plan to apply for Department of Veterans Affairs educational benefits based on my U.S. services affiliation identified above:</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Do you plan to use an education benefit or scholarship through an employer, corporation, foundation or other ASU education partner?</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Tigrigna</t>
+  </si>
+  <si>
+    <t>Test Address line1 Test Address line2
+TestTestTestTestTestTestTestTest,Brong-Ahafo,Ghana
+12345-678910</t>
+  </si>
+  <si>
+    <t>Test Address line1 Test Address line2
+Test City,Eastern,Ghana
+12345-678910</t>
+  </si>
+  <si>
+    <t>Spanish-Mexican</t>
+  </si>
+  <si>
+    <t>Mongolian</t>
+  </si>
+  <si>
+    <t>Bouvet Island</t>
+  </si>
+  <si>
+    <t>Parent or Legal Guardian Attended ASU</t>
+  </si>
+  <si>
+    <t>Grandparent</t>
+  </si>
+  <si>
+    <t>United States Air Force
+United States Army
+United States Marine Corps
+United States Navy
+United States Air Force
+United States Coast Guard
+United States Space Force
+United States Public Health Service Commissioned Corps
+National Oceanic and Atmospheric Administration Commissioned Officer Corps</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Current employer</t>
+  </si>
+  <si>
+    <t>City of phoenix</t>
   </si>
 </sst>
 </file>
@@ -426,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="67">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -449,6 +647,162 @@
       <alignment horizontal="left"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
@@ -3107,8 +3461,8 @@
       <c r="A1" t="s" s="0">
         <v>102</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>103</v>
+      <c r="B1" s="17" t="s">
+        <v>106</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
@@ -3119,8 +3473,12 @@
       <c r="L1" s="3"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="3"/>
+      <c r="A2" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>108</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="3"/>
@@ -3129,8 +3487,12 @@
       <c r="L2" s="3"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="3"/>
+      <c r="A3" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
       <c r="F3" s="3"/>
@@ -3139,8 +3501,12 @@
       <c r="L3" s="3"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="3"/>
+      <c r="A4" t="s" s="0">
+        <v>110</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>111</v>
+      </c>
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
       <c r="F4" s="3"/>
@@ -3178,8 +3544,12 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3"/>
+      <c r="A8" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>149</v>
+      </c>
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
       <c r="F8" s="3"/>
@@ -3188,8 +3558,12 @@
       <c r="L8" s="3"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="3"/>
+      <c r="A9" t="s" s="0">
+        <v>114</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>150</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
       <c r="F9" s="3"/>
@@ -3198,8 +3572,12 @@
       <c r="L9" s="3"/>
     </row>
     <row r="10" ht="137.25" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="3"/>
+      <c r="A10" t="s" s="0">
+        <v>116</v>
+      </c>
+      <c r="B10" s="46" t="s">
+        <v>152</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
       <c r="F10" s="3"/>
@@ -3231,8 +3609,12 @@
       <c r="L12" s="3"/>
     </row>
     <row r="13" ht="33.0" customHeight="1">
-      <c r="A13" s="4"/>
-      <c r="B13" s="3"/>
+      <c r="A13" t="s" s="0">
+        <v>119</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>154</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" s="4"/>
       <c r="F13" s="3"/>
@@ -3241,8 +3623,12 @@
       <c r="L13" s="3"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="4"/>
-      <c r="B14" s="3"/>
+      <c r="A14" t="s" s="0">
+        <v>122</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>123</v>
+      </c>
       <c r="D14" s="3"/>
       <c r="E14" s="4"/>
       <c r="F14" s="3"/>
@@ -3251,8 +3637,12 @@
       <c r="L14" s="3"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="4"/>
-      <c r="B15" s="3"/>
+      <c r="A15" t="s" s="0">
+        <v>124</v>
+      </c>
+      <c r="B15" s="50" t="s">
+        <v>125</v>
+      </c>
       <c r="D15" s="3"/>
       <c r="E15" s="4"/>
       <c r="F15" s="3"/>
@@ -3261,8 +3651,12 @@
       <c r="L15" s="3"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="4"/>
-      <c r="B16" s="3"/>
+      <c r="A16" t="s" s="0">
+        <v>126</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>155</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4"/>
       <c r="F16" s="3"/>
@@ -3271,8 +3665,12 @@
       <c r="L16" s="3"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="4"/>
-      <c r="B17" s="3"/>
+      <c r="A17" t="s" s="0">
+        <v>128</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>129</v>
+      </c>
       <c r="D17" s="3"/>
       <c r="E17" s="4"/>
       <c r="F17" s="3"/>
@@ -3289,47 +3687,80 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="3"/>
+      <c r="A19" t="s" s="0">
+        <v>130</v>
+      </c>
+      <c r="B19" s="54" t="s">
+        <v>131</v>
+      </c>
       <c r="H19" s="3"/>
       <c r="K19" s="4"/>
       <c r="L19" s="3"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="3"/>
+      <c r="A20" t="s" s="0">
+        <v>132</v>
+      </c>
+      <c r="B20" s="55" t="s">
+        <v>138</v>
+      </c>
       <c r="H20" s="3"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="4"/>
-      <c r="B21" s="3"/>
+      <c r="A21" t="s" s="0">
+        <v>134</v>
+      </c>
+      <c r="B21" s="56" t="s">
+        <v>135</v>
+      </c>
       <c r="H21" s="3"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="B22" s="3"/>
+      <c r="A22" t="s" s="0">
+        <v>156</v>
+      </c>
+      <c r="B22" s="53" t="s">
+        <v>147</v>
+      </c>
       <c r="H22" s="3"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="3"/>
+      <c r="A23" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="B23" s="57" t="s">
+        <v>137</v>
+      </c>
       <c r="H23" s="3"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="4"/>
-      <c r="B24" s="3"/>
+      <c r="A24" t="s" s="0">
+        <v>132</v>
+      </c>
+      <c r="B24" s="58" t="s">
+        <v>157</v>
+      </c>
       <c r="H24" s="3"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="4"/>
-      <c r="B25" s="3"/>
+      <c r="A25" t="s" s="0">
+        <v>134</v>
+      </c>
+      <c r="B25" s="59" t="s">
+        <v>139</v>
+      </c>
       <c r="H25" s="3"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="B26" s="3"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="4"/>
-      <c r="B27" s="3"/>
+      <c r="A27" t="s" s="0">
+        <v>140</v>
+      </c>
+      <c r="B27" s="60" t="s">
+        <v>141</v>
+      </c>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
       <c r="F27" s="3"/>
@@ -3348,8 +3779,12 @@
       <c r="L28" s="3"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="4"/>
-      <c r="B29" s="3"/>
+      <c r="A29" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="B29" s="61" t="s">
+        <v>143</v>
+      </c>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
       <c r="F29" s="3"/>
@@ -3359,8 +3794,12 @@
       <c r="L29" s="3"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="4"/>
-      <c r="B30" s="3"/>
+      <c r="A30" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="B30" s="62" t="s">
+        <v>158</v>
+      </c>
       <c r="D30" s="3"/>
       <c r="E30" s="4"/>
       <c r="F30" s="3"/>
@@ -3368,8 +3807,12 @@
       <c r="L30" s="3"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="4"/>
-      <c r="B31" s="3"/>
+      <c r="A31" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="B31" s="63" t="s">
+        <v>159</v>
+      </c>
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
       <c r="F31" s="3"/>
@@ -3385,8 +3828,12 @@
       <c r="L32" s="3"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="4"/>
-      <c r="B33" s="3"/>
+      <c r="A33" t="s" s="0">
+        <v>148</v>
+      </c>
+      <c r="B33" s="66" t="s">
+        <v>159</v>
+      </c>
       <c r="D33" s="3"/>
       <c r="E33" s="4"/>
       <c r="F33" s="3"/>
@@ -3395,8 +3842,12 @@
       <c r="L33" s="3"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="4"/>
-      <c r="B34" s="3"/>
+      <c r="A34" t="s" s="0">
+        <v>160</v>
+      </c>
+      <c r="B34" s="65" t="s">
+        <v>161</v>
+      </c>
       <c r="D34" s="3"/>
       <c r="E34" s="4"/>
       <c r="F34" s="3"/>

</xml_diff>

<commit_message>
F-1 to F-7 flows are complete
</commit_message>
<xml_diff>
--- a/UAA/src/src/test/resources/com/ugapp/excel/testdata.xlsx
+++ b/UAA/src/src/test/resources/com/ugapp/excel/testdata.xlsx
@@ -21,14 +21,13 @@
     <sheet state="visible" name="AddMaxHighSchoolTest" sheetId="13" r:id="rId16"/>
     <sheet state="visible" name="overAllAcademicsTest" sheetId="14" r:id="rId17"/>
     <sheet state="visible" name="CollegeUniversitiesTest" sheetId="15" r:id="rId18"/>
-    <sheet name="Mismatch_01_valid_vs_Revie" r:id="rId19" sheetId="16"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="106">
   <si>
     <t>TCID</t>
   </si>
@@ -339,797 +338,13 @@
     <t>Email</t>
   </si>
   <si>
-    <t>376290@test.asu.edu</t>
-  </si>
-  <si>
-    <t>Legal name</t>
-  </si>
-  <si>
-    <t>Test FN Automation MN Test LN</t>
-  </si>
-  <si>
-    <t>Preferred first name</t>
+    <t>112419@test.asu.edu</t>
   </si>
   <si>
     <t>Date of birth</t>
   </si>
   <si>
-    <t>June 21, 1973</t>
-  </si>
-  <si>
-    <t>Legal sex</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Primary language spoken at home</t>
-  </si>
-  <si>
-    <t>German, Standard</t>
-  </si>
-  <si>
-    <t>Home address</t>
-  </si>
-  <si>
-    <t>Test Address line1 Test Address line2
-TestTestTestTestTestTestTestTest,Al 'Asimah,Bahrain
-12345-678910</t>
-  </si>
-  <si>
-    <t>Test Address line1 Test Address line2
-Test City,Al Janubiyah,Bahrain
-12345-678910</t>
-  </si>
-  <si>
-    <t>U.S. citizenship</t>
-  </si>
-  <si>
-    <t>I am a U.S. citizen</t>
-  </si>
-  <si>
-    <t>Country of citizenship</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>Country of birth</t>
-  </si>
-  <si>
-    <t>Greece</t>
-  </si>
-  <si>
-    <t>Social Security Number</t>
-  </si>
-  <si>
-    <t>*********</t>
-  </si>
-  <si>
-    <t>Parent or Legal Guardian Attended ASU</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Parent or legal guardian</t>
-  </si>
-  <si>
-    <t>Parent FN Parent LN I</t>
-  </si>
-  <si>
-    <t>Parent or Legal Guardian Relation</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Parent or Legal Guardian Schooling Level</t>
-  </si>
-  <si>
-    <t>Other/Unknown</t>
-  </si>
-  <si>
-    <t>Additional parent or legal guardian</t>
-  </si>
-  <si>
-    <t>Parent FN Parent LN II</t>
-  </si>
-  <si>
-    <t>Father</t>
-  </si>
-  <si>
-    <t>College or Beyond</t>
-  </si>
-  <si>
-    <t>Previous ASU affiliation</t>
-  </si>
-  <si>
-    <t>I have never been affiliated with Arizona State University</t>
-  </si>
-  <si>
-    <t>Military status</t>
-  </si>
-  <si>
-    <t>I am the spouse/dependent of a U.S. service member or veteran</t>
-  </si>
-  <si>
-    <t>Branch</t>
-  </si>
-  <si>
-    <t>United States Army
-United States Army
-United States Marine Corps
-United States Navy
-United States Air Force
-United States Coast Guard
-United States Space Force
-United States Public Health Service Commissioned Corps
-National Oceanic and Atmospheric Administration Commissioned Officer Corps</t>
-  </si>
-  <si>
-    <t>I have applied or plan to apply for Department of Veterans Affairs educational benefits based on my U.S. services affiliation identified above:</t>
-  </si>
-  <si>
-    <t>Do you plan to use an education benefit or scholarship through an employer, corporation, foundation or other ASU education partner?</t>
-  </si>
-  <si>
-    <t>Current employer</t>
-  </si>
-  <si>
-    <t>Gila river gaming</t>
-  </si>
-  <si>
-    <t>Pre-law interest</t>
-  </si>
-  <si>
-    <t>Pre-med/health interest</t>
-  </si>
-  <si>
-    <t>Pre-veterinary interest</t>
-  </si>
-  <si>
-    <t>Teaching certificate interest</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Graduating school </t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>High school name</t>
-  </si>
-  <si>
-    <t>Pace Preparatory Academy</t>
-  </si>
-  <si>
-    <t>Name on transcript</t>
-  </si>
-  <si>
-    <t>Test FN Test LN</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Humboldt, Arizona
-Alabama
-Alaska
-American Samoa
-Arizona
-Arkansas
-Armed Forces Americas
-Armed Forces Europe
-Armed Forces Pacific
-California
-Colorado
-Connecticut
-Delaware
-District of Columbia
-Florida
-Georgia
-Guam Federal
-Hawaii
-Idaho
-Illinois
-Indiana
-Iowa
-Kansas
-Kentucky
-Louisiana
-Maine
-Maryland
-Massachusetts
-Michigan
-Minnesota
-Mississippi
-Missouri
-Montana
-Nebraska
-Nevada
-New Hampshire
-New Jersey
-New Mexico
-New York
-North Carolina
-North Dakota
-Northern Mariana Islands
-Ohio
-Oklahoma
-Oregon
-Pennsylvania
-Puerto Rico Federal
-Rhode Island
-South Carolina
-South Dakota
-Tennessee
-Texas
-Utah
-Vermont
-Virgin Islands
-Virginia
-Washington
-West Virginia
-Wisconsin
-Wyoming, USA</t>
-  </si>
-  <si>
-    <t>Graduation date</t>
-  </si>
-  <si>
-    <t>October, 2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Past schools </t>
-  </si>
-  <si>
-    <t>Date first attended</t>
-  </si>
-  <si>
-    <t>May, 1971</t>
-  </si>
-  <si>
-    <t>Date last attended</t>
-  </si>
-  <si>
-    <t>January, 1989
-2024
-2023
-2022
-2021
-2020
-2019
-2018
-2017
-2016
-2015
-2014
-2013
-2012
-2011
-2010
-2009
-2008
-2007
-2006
-2005
-2004
-2003
-2002
-2001
-2000
-1999
-1998
-1997
-1996
-1995
-1994
-1993
-1992
-1991
-1990
-1989
-1988
-1987
-1986
-1985
-1984
-1983
-1982
-1981
-1980
-1979
-1978
-1977
-1976
-1975
-1974
-1973
-1972
-1971
-1970
-1969
-1968
-1967
-1966
-1965
-1964
-1963
-1962
-1961
-1960
-1959
-1958
-1957
-1956
-1955
-1954
-1953
-1952
-1951
-1950
-1949
-1948
-1947
-1946
-1945
-1944
-1943
-1942
-1941
-1940
-1939
-1938
-1937
-1936
-1935
-1934
-1933
-1932
-1931
-1930
-1929
-1928
-1927
-1926
-1925
-1924</t>
-  </si>
-  <si>
-    <t>are you eligible to return to each of the colleges or universities you have attended in the last seven years?</t>
-  </si>
-  <si>
-    <t>Unweighted GPA/Scale</t>
-  </si>
-  <si>
-    <t>1 / 100</t>
-  </si>
-  <si>
-    <t>Grading system</t>
-  </si>
-  <si>
-    <t>100 point based</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>No data has been entered</t>
-  </si>
-  <si>
-    <t>Math</t>
-  </si>
-  <si>
-    <t>Science</t>
-  </si>
-  <si>
-    <t>Social Science</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>Fine Arts/CTE</t>
-  </si>
-  <si>
-    <t>OTHER TEST</t>
-  </si>
-  <si>
-    <t>Electives</t>
-  </si>
-  <si>
-    <t>Band</t>
-  </si>
-  <si>
-    <t>Begin by selecting the state you consider to be your permanent home.</t>
-  </si>
-  <si>
-    <t>Outside the U.S. or Not Listed</t>
-  </si>
-  <si>
-    <t>Are you currently enrolled at another college or university?</t>
-  </si>
-  <si>
-    <t>Where are you currently enrolled?</t>
-  </si>
-  <si>
-    <t>Test College</t>
-  </si>
-  <si>
-    <t>In which state is that school located?</t>
-  </si>
-  <si>
-    <t>Maryland</t>
-  </si>
-  <si>
-    <t>Were you enrolled at any Arizona college or university in 2024 or 2023 calendar year?</t>
-  </si>
-  <si>
-    <t>Do you have a current driver’s license or state issued ID?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> In which state was your license issued? </t>
-  </si>
-  <si>
-    <t>Arizona</t>
-  </si>
-  <si>
-    <t>When was your license issued?</t>
-  </si>
-  <si>
-    <t>1939-12</t>
-  </si>
-  <si>
-    <t>Do you own or operate a car, motorcycle or other motor vehicle?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Is this vehicle registered in the state of Arizona? </t>
-  </si>
-  <si>
-    <t>When was your vehicle registered?</t>
-  </si>
-  <si>
-    <t>1987-03</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Did you, or will you, file state taxes for 2022? </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Where did or where will you file your state taxes for 2022? </t>
-  </si>
-  <si>
-    <t>Arkansas</t>
-  </si>
-  <si>
-    <t>Parent or legal guardian financial support</t>
-  </si>
-  <si>
-    <t>86</t>
-  </si>
-  <si>
-    <t>Employment financial support</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Financial aid financial support</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Spouse financial support</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Other financial support</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Savings/trust fund financial support</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Retirement financial support</t>
-  </si>
-  <si>
-    <t>Social Security/Disability financial support</t>
-  </si>
-  <si>
-    <t>Veteran Benefits financial support</t>
-  </si>
-  <si>
-    <t>State or Federal Benefits financial support</t>
-  </si>
-  <si>
-    <t>Unemployment financial support</t>
-  </si>
-  <si>
-    <t>Other/none of the above financial support</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Are you currently employed? </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Where is your primary work location? </t>
-  </si>
-  <si>
-    <t>When did your employment at this location begin?</t>
-  </si>
-  <si>
-    <t>1952-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> You indicated that you were the spouse or dependent of a U.S. service member or veteran. Which best describes the service member or veteran? </t>
-  </si>
-  <si>
-    <t>Active Duty</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Where is your spouse/parent/guardian currently stationed? </t>
-  </si>
-  <si>
-    <t>Northern Mariana Islands</t>
-  </si>
-  <si>
-    <t>What is your spouse/parent/guardians state of legal residence?</t>
-  </si>
-  <si>
-    <t>Guam Federal</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> In which state do your parent(s) or legal guardian(s) currently live? </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Which parent or legal guardian lives in Arizona? </t>
-  </si>
-  <si>
-    <t>Both</t>
-  </si>
-  <si>
-    <t>When did your parent(s) or legal guardian(s) begin living in Arizona continuously?</t>
-  </si>
-  <si>
-    <t>June-null</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Did or will your parent(s) or legal guardian(s) file a state income tax return for the 2022 tax year? </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> In which state did, or will, your parent(s) or legal guardian(s) file state income taxes? </t>
-  </si>
-  <si>
-    <t>Wyoming</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Does either parent or legal guardian have a current Arizona driver license? </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Is either parent or legal guardian employed in Arizona? </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> In which state does your spouse currently live? </t>
-  </si>
-  <si>
-    <t>When did your spouse begin living in Arizona?</t>
-  </si>
-  <si>
-    <t>1963-07</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Does your spouse have a valid drivers license or state-issued ID? </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> What state issued this drivers license or state ID?  </t>
-  </si>
-  <si>
-    <t>When did your spouse obtain this drivers license or state ID?</t>
-  </si>
-  <si>
-    <t>2016-05</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Did or will your spouse file a state income tax return for the 2022 tax year? </t>
-  </si>
-  <si>
-    <t>In which state did, or will, your spouse file state income taxes?</t>
-  </si>
-  <si>
-    <t>District of Columbia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Is your spouse employed? </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> In which state is your spouse employed? </t>
-  </si>
-  <si>
-    <t>When did your spouses employment at this location begin?</t>
-  </si>
-  <si>
-    <t>1983-10</t>
-  </si>
-  <si>
-    <t>Is your spouse currently enrolled at ASU or any other college or university?</t>
-  </si>
-  <si>
-    <t>Is your spouse dependent on someone other than you for financial support, e.g. parents, guardians, family or financial aid?</t>
-  </si>
-  <si>
-    <t>Pronouns</t>
-  </si>
-  <si>
-    <t>She/Her</t>
-  </si>
-  <si>
-    <t>Gender identity</t>
-  </si>
-  <si>
-    <t>Identity not listed</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>+12642351234</t>
-  </si>
-  <si>
-    <t>Mobile phone</t>
-  </si>
-  <si>
-    <t>+93701234567</t>
-  </si>
-  <si>
-    <t>Mobile SMS</t>
-  </si>
-  <si>
-    <t>Former name(s)</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Ethnic/racial background</t>
-  </si>
-  <si>
-    <t>Affiliate ID</t>
-  </si>
-  <si>
-    <t>United States Army</t>
-  </si>
-  <si>
-    <t>First choice</t>
-  </si>
-  <si>
-    <t>African and African American Studies, BA</t>
-  </si>
-  <si>
-    <t>Tempe</t>
-  </si>
-  <si>
-    <t>Starting term</t>
-  </si>
-  <si>
-    <t>Summer 2025 - (Session C)</t>
-  </si>
-  <si>
-    <t>Graduating school</t>
-  </si>
-  <si>
-    <t>Humboldt, AZ, USA</t>
-  </si>
-  <si>
-    <t>Past colleges/universities</t>
-  </si>
-  <si>
-    <t>School name</t>
-  </si>
-  <si>
-    <t>Test City, EE, SSD</t>
-  </si>
-  <si>
-    <t>Degree</t>
-  </si>
-  <si>
-    <t>Associate of Arts</t>
-  </si>
-  <si>
-    <t>Degree concentration</t>
-  </si>
-  <si>
-    <t>January, 1989</t>
-  </si>
-  <si>
-    <t>Transfer credits to ASU</t>
-  </si>
-  <si>
-    <t>Are you eligible to return to each of the colleges or universities you have attended in the last seven years? If you have not attended college, please answer yes.</t>
-  </si>
-  <si>
-    <t>Self-reported</t>
-  </si>
-  <si>
-    <t>Is this vehicle registered in the state of Arizona?</t>
-  </si>
-  <si>
-    <t>In which state was your license issued?</t>
-  </si>
-  <si>
-    <t>Did you, or will you, file state taxes for 2023?</t>
-  </si>
-  <si>
-    <t>Where did or where will you file your state taxes for 2023?</t>
-  </si>
-  <si>
-    <t>Other/none of the above</t>
-  </si>
-  <si>
-    <t>Are you currently employed?</t>
-  </si>
-  <si>
-    <t>Where is your primary work location?</t>
-  </si>
-  <si>
-    <t>In which state do your parent(s) or legal guardian(s) currently live?</t>
-  </si>
-  <si>
-    <t>Which parent or legal guardian lives in Arizona?</t>
-  </si>
-  <si>
-    <t>Did or will your parent(s) or legal guardian(s) file a state income tax return for the 2023 tax year?</t>
-  </si>
-  <si>
-    <t>In which state did, or will, your parent(s) or legal guardian(s) file state income taxes?</t>
-  </si>
-  <si>
-    <t>Does either parent or legal guardian have a current Arizona driver license?</t>
-  </si>
-  <si>
-    <t>Is either parent or legal guardian employed in Arizona?</t>
-  </si>
-  <si>
-    <t>In which state does your spouse currently live?</t>
-  </si>
-  <si>
-    <t>Does your spouse have a valid drivers license or state-issued ID?</t>
-  </si>
-  <si>
-    <t>What state issued this drivers license or state ID?</t>
-  </si>
-  <si>
-    <t>Is your spouse employed?</t>
-  </si>
-  <si>
-    <t>In which state is your spouse employed?</t>
-  </si>
-  <si>
-    <t>Did or will your spouse file a state income tax return for the 2023 tax year?</t>
-  </si>
-  <si>
-    <t>You indicated that you were the spouse or dependent of a U.S. service member or veteran. Which best describes the service member or veteran?</t>
-  </si>
-  <si>
-    <t>Where is your spouse/parent/guardian currently stationed?</t>
-  </si>
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>Value Sheet 1</t>
-  </si>
-  <si>
-    <t>Value Sheet 2</t>
+    <t>May 24, 1988</t>
   </si>
 </sst>
 </file>
@@ -1217,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="240">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1240,678 +455,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
@@ -4548,63 +3091,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>307</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>308</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>164</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>165</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>141</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>157</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>158</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>278</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -4642,12 +3128,8 @@
       <c r="L1" s="3"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="0">
-        <v>104</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>105</v>
-      </c>
+      <c r="A2" s="4"/>
+      <c r="B2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="3"/>
@@ -4656,12 +3138,8 @@
       <c r="L2" s="3"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>29</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
       <c r="F3" s="3"/>
@@ -4671,10 +3149,10 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="0">
-        <v>107</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>108</v>
+        <v>104</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>105</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
@@ -4684,12 +3162,8 @@
       <c r="L4" s="3"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" t="s" s="0">
-        <v>255</v>
-      </c>
-      <c r="B5" s="124" t="s">
-        <v>256</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="4"/>
       <c r="F5" s="3"/>
@@ -4700,12 +3174,8 @@
       <c r="L5" s="3"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" t="s" s="0">
-        <v>257</v>
-      </c>
-      <c r="B6" s="125" t="s">
-        <v>258</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="4"/>
       <c r="F6" s="3"/>
@@ -4721,12 +3191,8 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" t="s" s="0">
-        <v>109</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>110</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
       <c r="F8" s="3"/>
@@ -4735,12 +3201,8 @@
       <c r="L8" s="3"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" t="s" s="0">
-        <v>111</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>112</v>
-      </c>
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
       <c r="F9" s="3"/>
@@ -4749,12 +3211,8 @@
       <c r="L9" s="3"/>
     </row>
     <row r="10" ht="137.25" customHeight="1">
-      <c r="A10" t="s" s="0">
-        <v>113</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>115</v>
-      </c>
+      <c r="A10" s="4"/>
+      <c r="B10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
       <c r="F10" s="3"/>
@@ -4796,12 +3254,8 @@
       <c r="L13" s="3"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" t="s" s="0">
-        <v>116</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>117</v>
-      </c>
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="4"/>
       <c r="F14" s="3"/>
@@ -4810,12 +3264,8 @@
       <c r="L14" s="3"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" t="s" s="0">
-        <v>118</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>119</v>
-      </c>
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="4"/>
       <c r="F15" s="3"/>
@@ -4824,12 +3274,8 @@
       <c r="L15" s="3"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" t="s" s="0">
-        <v>120</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>121</v>
-      </c>
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="4"/>
       <c r="F16" s="3"/>
@@ -4838,12 +3284,8 @@
       <c r="L16" s="3"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" t="s" s="0">
-        <v>122</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>123</v>
-      </c>
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="4"/>
       <c r="F17" s="3"/>
@@ -4860,80 +3302,47 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" t="s" s="0">
-        <v>127</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>128</v>
-      </c>
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
       <c r="H19" s="3"/>
       <c r="K19" s="4"/>
       <c r="L19" s="3"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" t="s" s="0">
-        <v>129</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>130</v>
-      </c>
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
       <c r="H20" s="3"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" t="s" s="0">
-        <v>131</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>132</v>
-      </c>
+      <c r="A21" s="4"/>
+      <c r="B21" s="3"/>
       <c r="H21" s="3"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" t="s" s="0">
-        <v>124</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>126</v>
-      </c>
+      <c r="B22" s="3"/>
       <c r="H22" s="3"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" t="s" s="0">
-        <v>133</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>134</v>
-      </c>
+      <c r="A23" s="4"/>
+      <c r="B23" s="3"/>
       <c r="H23" s="3"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" t="s" s="0">
-        <v>129</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>135</v>
-      </c>
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
       <c r="H24" s="3"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" t="s" s="0">
-        <v>131</v>
-      </c>
-      <c r="B25" s="33" t="s">
-        <v>136</v>
-      </c>
+      <c r="A25" s="4"/>
+      <c r="B25" s="3"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="B26" s="3"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" t="s" s="0">
-        <v>137</v>
-      </c>
-      <c r="B27" s="34" t="s">
-        <v>138</v>
-      </c>
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
       <c r="F27" s="3"/>
@@ -4952,12 +3361,8 @@
       <c r="L28" s="3"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" t="s" s="0">
-        <v>139</v>
-      </c>
-      <c r="B29" s="35" t="s">
-        <v>140</v>
-      </c>
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
       <c r="F29" s="3"/>
@@ -4967,12 +3372,8 @@
       <c r="L29" s="3"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" t="s" s="0">
-        <v>141</v>
-      </c>
-      <c r="B30" s="36" t="s">
-        <v>142</v>
-      </c>
+      <c r="A30" s="4"/>
+      <c r="B30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="4"/>
       <c r="F30" s="3"/>
@@ -4980,12 +3381,8 @@
       <c r="L30" s="3"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" t="s" s="0">
-        <v>143</v>
-      </c>
-      <c r="B31" s="37" t="s">
-        <v>126</v>
-      </c>
+      <c r="A31" s="4"/>
+      <c r="B31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
       <c r="F31" s="3"/>
@@ -5001,12 +3398,8 @@
       <c r="L32" s="3"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" t="s" s="0">
-        <v>144</v>
-      </c>
-      <c r="B33" s="40" t="s">
-        <v>125</v>
-      </c>
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="4"/>
       <c r="F33" s="3"/>
@@ -5015,12 +3408,8 @@
       <c r="L33" s="3"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" t="s" s="0">
-        <v>145</v>
-      </c>
-      <c r="B34" s="39" t="s">
-        <v>146</v>
-      </c>
+      <c r="A34" s="4"/>
+      <c r="B34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="4"/>
       <c r="F34" s="3"/>
@@ -5090,12 +3479,8 @@
       <c r="J40" s="3"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" t="s" s="0">
-        <v>147</v>
-      </c>
-      <c r="B41" s="41" t="s">
-        <v>126</v>
-      </c>
+      <c r="A41" s="4"/>
+      <c r="B41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="4"/>
       <c r="F41" s="3"/>
@@ -5106,12 +3491,8 @@
       <c r="L41" s="3"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" t="s" s="0">
-        <v>148</v>
-      </c>
-      <c r="B42" s="42" t="s">
-        <v>125</v>
-      </c>
+      <c r="A42" s="4"/>
+      <c r="B42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="4"/>
       <c r="F42" s="3"/>
@@ -5122,12 +3503,8 @@
       <c r="L42" s="3"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" t="s" s="0">
-        <v>149</v>
-      </c>
-      <c r="B43" s="43" t="s">
-        <v>125</v>
-      </c>
+      <c r="A43" s="4"/>
+      <c r="B43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="4"/>
       <c r="F43" s="3"/>
@@ -5138,12 +3515,8 @@
       <c r="L43" s="3"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" t="s" s="0">
-        <v>150</v>
-      </c>
-      <c r="B44" s="44" t="s">
-        <v>126</v>
-      </c>
+      <c r="A44" s="4"/>
+      <c r="B44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="4"/>
       <c r="F44" s="3"/>
@@ -5154,12 +3527,8 @@
       <c r="L44" s="3"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" t="s" s="0">
-        <v>151</v>
-      </c>
-      <c r="B45" s="45" t="s">
-        <v>152</v>
-      </c>
+      <c r="A45" s="4"/>
+      <c r="B45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="4"/>
       <c r="F45" s="3"/>
@@ -5170,12 +3539,8 @@
       <c r="L45" s="3"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" t="s" s="0">
-        <v>153</v>
-      </c>
-      <c r="B46" s="46" t="s">
-        <v>154</v>
-      </c>
+      <c r="A46" s="4"/>
+      <c r="B46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="4"/>
       <c r="F46" s="3"/>
@@ -5186,12 +3551,8 @@
       <c r="L46" s="3"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" t="s" s="0">
-        <v>155</v>
-      </c>
-      <c r="B47" s="47" t="s">
-        <v>156</v>
-      </c>
+      <c r="A47" s="4"/>
+      <c r="B47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="4"/>
       <c r="F47" s="3"/>
@@ -5202,12 +3563,8 @@
       <c r="L47" s="3"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" t="s" s="0">
-        <v>157</v>
-      </c>
-      <c r="B48" s="48" t="s">
-        <v>158</v>
-      </c>
+      <c r="A48" s="4"/>
+      <c r="B48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="4"/>
       <c r="F48" s="3"/>
@@ -5218,12 +3575,8 @@
       <c r="L48" s="3"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" t="s" s="0">
-        <v>159</v>
-      </c>
-      <c r="B49" s="49" t="s">
-        <v>160</v>
-      </c>
+      <c r="A49" s="4"/>
+      <c r="B49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="4"/>
       <c r="F49" s="3"/>
@@ -5234,12 +3587,8 @@
       <c r="L49" s="3"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" t="s" s="0">
-        <v>161</v>
-      </c>
-      <c r="B50" s="50" t="s">
-        <v>152</v>
-      </c>
+      <c r="A50" s="4"/>
+      <c r="B50" s="3"/>
       <c r="D50" s="3"/>
       <c r="H50" s="3"/>
     </row>
@@ -5536,12 +3885,8 @@
       <c r="L101" s="3"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
-      <c r="A102" t="s" s="0">
-        <v>162</v>
-      </c>
-      <c r="B102" s="51" t="s">
-        <v>163</v>
-      </c>
+      <c r="A102" s="4"/>
+      <c r="B102" s="3"/>
       <c r="E102" s="4"/>
       <c r="F102" s="3"/>
       <c r="H102" s="3"/>
@@ -5551,12 +3896,8 @@
       <c r="L102" s="3"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
-      <c r="A103" t="s" s="0">
-        <v>164</v>
-      </c>
-      <c r="B103" s="52" t="s">
-        <v>165</v>
-      </c>
+      <c r="A103" s="4"/>
+      <c r="B103" s="3"/>
       <c r="E103" s="4"/>
       <c r="F103" s="3"/>
       <c r="H103" s="3"/>
@@ -5577,12 +3918,8 @@
       <c r="L104" s="3"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
-      <c r="A105" t="s" s="0">
-        <v>166</v>
-      </c>
-      <c r="B105" s="53" t="s">
-        <v>125</v>
-      </c>
+      <c r="A105" s="4"/>
+      <c r="B105" s="3"/>
       <c r="E105" s="4"/>
       <c r="F105" s="3"/>
       <c r="H105" s="3"/>
@@ -5679,23 +4016,15 @@
       <c r="H115" s="3"/>
     </row>
     <row r="116" ht="14.25" customHeight="1">
-      <c r="A116" t="s" s="0">
-        <v>167</v>
-      </c>
-      <c r="B116" s="65" t="s">
-        <v>168</v>
-      </c>
+      <c r="A116" s="4"/>
+      <c r="B116" s="3"/>
       <c r="E116" s="4"/>
       <c r="F116" s="3"/>
       <c r="H116" s="3"/>
     </row>
     <row r="117" ht="14.25" customHeight="1">
-      <c r="A117" t="s" s="0">
-        <v>232</v>
-      </c>
-      <c r="B117" s="107" t="s">
-        <v>233</v>
-      </c>
+      <c r="A117" s="4"/>
+      <c r="B117" s="3"/>
       <c r="E117" s="4"/>
       <c r="F117" s="3"/>
       <c r="H117" s="3"/>
@@ -5708,82 +4037,50 @@
       <c r="H118" s="3"/>
     </row>
     <row r="119" ht="14.25" customHeight="1">
-      <c r="A119" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="B119" s="67" t="s">
-        <v>172</v>
-      </c>
+      <c r="A119" s="4"/>
+      <c r="B119" s="3"/>
       <c r="E119" s="4"/>
       <c r="F119" s="3"/>
     </row>
     <row r="120" ht="14.25" customHeight="1">
-      <c r="A120" t="s" s="0">
-        <v>173</v>
-      </c>
-      <c r="B120" s="68" t="s">
-        <v>172</v>
-      </c>
+      <c r="A120" s="4"/>
+      <c r="B120" s="3"/>
       <c r="E120" s="4"/>
       <c r="F120" s="3"/>
     </row>
     <row r="121" ht="14.25" customHeight="1">
-      <c r="A121" t="s" s="0">
-        <v>174</v>
-      </c>
-      <c r="B121" s="69" t="s">
-        <v>172</v>
-      </c>
+      <c r="A121" s="4"/>
+      <c r="B121" s="3"/>
       <c r="E121" s="4"/>
       <c r="F121" s="3"/>
     </row>
     <row r="122" ht="14.25" customHeight="1">
-      <c r="A122" t="s" s="0">
-        <v>175</v>
-      </c>
-      <c r="B122" s="70" t="s">
-        <v>172</v>
-      </c>
+      <c r="A122" s="4"/>
+      <c r="B122" s="3"/>
       <c r="E122" s="4"/>
       <c r="F122" s="3"/>
     </row>
     <row r="123" ht="14.25" customHeight="1">
-      <c r="A123" t="s" s="0">
-        <v>176</v>
-      </c>
-      <c r="B123" s="71" t="s">
-        <v>172</v>
-      </c>
+      <c r="A123" s="4"/>
+      <c r="B123" s="3"/>
       <c r="E123" s="4"/>
       <c r="F123" s="3"/>
     </row>
     <row r="124" ht="14.25" customHeight="1">
-      <c r="A124" t="s" s="0">
-        <v>177</v>
-      </c>
-      <c r="B124" s="72" t="s">
-        <v>180</v>
-      </c>
+      <c r="A124" s="4"/>
+      <c r="B124" s="3"/>
       <c r="E124" s="4"/>
       <c r="F124" s="3"/>
     </row>
     <row r="125" ht="14.25" customHeight="1">
-      <c r="A125" t="s" s="0">
-        <v>179</v>
-      </c>
-      <c r="B125" s="73" t="s">
-        <v>172</v>
-      </c>
+      <c r="A125" s="4"/>
+      <c r="B125" s="3"/>
       <c r="E125" s="4"/>
       <c r="F125" s="3"/>
     </row>
     <row r="126" ht="14.25" customHeight="1">
-      <c r="A126" t="s" s="0">
-        <v>181</v>
-      </c>
-      <c r="B126" s="74" t="s">
-        <v>182</v>
-      </c>
+      <c r="A126" s="4"/>
+      <c r="B126" s="3"/>
       <c r="D126" s="3"/>
       <c r="E126" s="4"/>
       <c r="F126" s="3"/>
@@ -5799,42 +4096,26 @@
       <c r="F128" s="3"/>
     </row>
     <row r="129" ht="14.25" customHeight="1">
-      <c r="A129" t="s" s="0">
-        <v>183</v>
-      </c>
-      <c r="B129" s="75" t="s">
-        <v>125</v>
-      </c>
+      <c r="A129" s="4"/>
+      <c r="B129" s="3"/>
       <c r="E129" s="4"/>
       <c r="F129" s="3"/>
     </row>
     <row r="130" ht="14.25" customHeight="1">
-      <c r="A130" t="s" s="0">
-        <v>184</v>
-      </c>
-      <c r="B130" s="76" t="s">
-        <v>185</v>
-      </c>
+      <c r="A130" s="4"/>
+      <c r="B130" s="3"/>
       <c r="E130" s="4"/>
       <c r="F130" s="3"/>
     </row>
     <row r="131" ht="14.25" customHeight="1">
-      <c r="A131" t="s" s="0">
-        <v>186</v>
-      </c>
-      <c r="B131" s="77" t="s">
-        <v>187</v>
-      </c>
+      <c r="A131" s="4"/>
+      <c r="B131" s="3"/>
       <c r="E131" s="4"/>
       <c r="F131" s="3"/>
     </row>
     <row r="132" ht="14.25" customHeight="1">
-      <c r="A132" t="s" s="0">
-        <v>188</v>
-      </c>
-      <c r="B132" s="78" t="s">
-        <v>125</v>
-      </c>
+      <c r="A132" s="4"/>
+      <c r="B132" s="3"/>
       <c r="E132" s="4"/>
       <c r="F132" s="3"/>
     </row>
@@ -5864,227 +4145,131 @@
       <c r="F137" s="3"/>
     </row>
     <row r="138" ht="14.25" customHeight="1">
-      <c r="A138" t="s" s="0">
-        <v>189</v>
-      </c>
-      <c r="B138" s="79" t="s">
-        <v>125</v>
-      </c>
+      <c r="A138" s="4"/>
+      <c r="B138" s="3"/>
     </row>
     <row r="139" ht="14.25" customHeight="1">
-      <c r="A139" t="s" s="0">
-        <v>190</v>
-      </c>
-      <c r="B139" s="80" t="s">
-        <v>191</v>
-      </c>
+      <c r="A139" s="4"/>
+      <c r="B139" s="3"/>
     </row>
     <row r="140" ht="14.25" customHeight="1">
-      <c r="A140" t="s" s="0">
-        <v>192</v>
-      </c>
-      <c r="B140" s="81" t="s">
-        <v>193</v>
-      </c>
+      <c r="A140" s="4"/>
+      <c r="B140" s="3"/>
     </row>
     <row r="141" ht="14.25" customHeight="1">
-      <c r="A141" t="s" s="0">
-        <v>194</v>
-      </c>
-      <c r="B141" s="82" t="s">
-        <v>125</v>
-      </c>
+      <c r="A141" s="4"/>
+      <c r="B141" s="3"/>
       <c r="E141" s="4"/>
       <c r="F141" s="3"/>
     </row>
     <row r="142" ht="14.25" customHeight="1">
-      <c r="A142" t="s" s="0">
-        <v>195</v>
-      </c>
-      <c r="B142" s="83" t="s">
-        <v>125</v>
-      </c>
+      <c r="A142" s="4"/>
+      <c r="B142" s="3"/>
       <c r="E142" s="4"/>
       <c r="F142" s="3"/>
     </row>
     <row r="143" ht="14.25" customHeight="1">
-      <c r="A143" t="s" s="0">
-        <v>196</v>
-      </c>
-      <c r="B143" s="84" t="s">
-        <v>197</v>
-      </c>
+      <c r="A143" s="4"/>
+      <c r="B143" s="3"/>
       <c r="E143" s="4"/>
       <c r="F143" s="3"/>
     </row>
     <row r="144" ht="14.25" customHeight="1">
-      <c r="A144" t="s" s="0">
-        <v>198</v>
-      </c>
-      <c r="B144" s="85" t="s">
-        <v>125</v>
-      </c>
+      <c r="A144" s="4"/>
+      <c r="B144" s="3"/>
       <c r="E144" s="4"/>
       <c r="F144" s="3"/>
     </row>
     <row r="145" ht="14.25" customHeight="1">
-      <c r="A145" t="s" s="0">
-        <v>201</v>
-      </c>
-      <c r="B145" s="87" t="s">
-        <v>202</v>
-      </c>
+      <c r="A145" s="4"/>
+      <c r="B145" s="3"/>
     </row>
     <row r="146" ht="14.25" customHeight="1">
-      <c r="A146" t="s" s="0">
-        <v>203</v>
-      </c>
-      <c r="B146" s="88" t="s">
-        <v>204</v>
-      </c>
+      <c r="A146" s="4"/>
+      <c r="B146" s="3"/>
     </row>
     <row r="147" ht="14.25" customHeight="1">
-      <c r="A147" t="s" s="0">
-        <v>205</v>
-      </c>
-      <c r="B147" s="89" t="s">
-        <v>206</v>
-      </c>
+      <c r="A147" s="4"/>
+      <c r="B147" s="3"/>
     </row>
     <row r="148" ht="14.25" customHeight="1">
-      <c r="A148" t="s" s="0">
-        <v>207</v>
-      </c>
-      <c r="B148" s="90" t="s">
-        <v>208</v>
-      </c>
+      <c r="A148" s="4"/>
+      <c r="B148" s="3"/>
     </row>
     <row r="149" ht="14.25" customHeight="1">
-      <c r="A149" t="s" s="0">
-        <v>209</v>
-      </c>
-      <c r="B149" s="91" t="s">
-        <v>210</v>
-      </c>
+      <c r="A149" s="4"/>
+      <c r="B149" s="3"/>
     </row>
     <row r="150" ht="14.25" customHeight="1">
       <c r="B150" s="3"/>
     </row>
     <row r="151" ht="14.25" customHeight="1">
-      <c r="A151" t="s" s="0">
-        <v>211</v>
-      </c>
-      <c r="B151" s="92" t="s">
-        <v>212</v>
-      </c>
+      <c r="A151" s="4"/>
+      <c r="B151" s="3"/>
       <c r="E151" s="4"/>
       <c r="F151" s="3"/>
     </row>
     <row r="152" ht="14.25" customHeight="1">
-      <c r="A152" t="s" s="0">
-        <v>213</v>
-      </c>
-      <c r="B152" s="93" t="s">
-        <v>212</v>
-      </c>
+      <c r="A152" s="4"/>
+      <c r="B152" s="3"/>
       <c r="E152" s="4"/>
       <c r="F152" s="3"/>
     </row>
     <row r="153" ht="14.25" customHeight="1">
-      <c r="A153" t="s" s="0">
-        <v>214</v>
-      </c>
-      <c r="B153" s="94" t="s">
-        <v>212</v>
-      </c>
+      <c r="A153" s="4"/>
+      <c r="B153" s="3"/>
       <c r="E153" s="4"/>
       <c r="F153" s="3"/>
     </row>
     <row r="154" ht="14.25" customHeight="1">
-      <c r="A154" t="s" s="0">
-        <v>215</v>
-      </c>
-      <c r="B154" s="95" t="s">
-        <v>212</v>
-      </c>
+      <c r="A154" s="4"/>
+      <c r="B154" s="3"/>
       <c r="E154" s="4"/>
       <c r="F154" s="3"/>
     </row>
     <row r="155" ht="14.25" customHeight="1">
-      <c r="A155" t="s" s="0">
-        <v>216</v>
-      </c>
-      <c r="B155" s="96" t="s">
-        <v>3</v>
-      </c>
+      <c r="A155" s="4"/>
+      <c r="B155" s="3"/>
       <c r="E155" s="4"/>
       <c r="F155" s="3"/>
     </row>
     <row r="156" ht="14.25" customHeight="1">
-      <c r="A156" t="s" s="0">
-        <v>217</v>
-      </c>
-      <c r="B156" s="97" t="s">
-        <v>212</v>
-      </c>
+      <c r="A156" s="4"/>
+      <c r="B156" s="3"/>
       <c r="E156" s="4"/>
       <c r="F156" s="3"/>
     </row>
     <row r="157" ht="14.25" customHeight="1">
-      <c r="A157" t="s" s="0">
-        <v>218</v>
-      </c>
-      <c r="B157" s="98" t="s">
-        <v>212</v>
-      </c>
+      <c r="A157" s="4"/>
+      <c r="B157" s="3"/>
       <c r="E157" s="4"/>
       <c r="F157" s="3"/>
     </row>
     <row r="158" ht="14.25" customHeight="1">
-      <c r="A158" t="s" s="0">
-        <v>219</v>
-      </c>
-      <c r="B158" s="99" t="s">
-        <v>125</v>
-      </c>
+      <c r="A158" s="4"/>
+      <c r="B158" s="3"/>
       <c r="E158" s="4"/>
       <c r="F158" s="3"/>
     </row>
     <row r="159" ht="14.25" customHeight="1">
-      <c r="A159" t="s" s="0">
-        <v>220</v>
-      </c>
-      <c r="B159" s="100" t="s">
-        <v>191</v>
-      </c>
+      <c r="A159" s="4"/>
+      <c r="B159" s="3"/>
       <c r="E159" s="4"/>
       <c r="F159" s="3"/>
     </row>
     <row r="160" ht="14.25" customHeight="1">
-      <c r="A160" t="s" s="0">
-        <v>223</v>
-      </c>
-      <c r="B160" s="102" t="s">
-        <v>224</v>
-      </c>
+      <c r="A160" s="4"/>
+      <c r="B160" s="3"/>
       <c r="E160" s="4"/>
       <c r="F160" s="3"/>
     </row>
     <row r="161" ht="14.25" customHeight="1">
-      <c r="A161" t="s" s="0">
-        <v>225</v>
-      </c>
-      <c r="B161" s="103" t="s">
-        <v>226</v>
-      </c>
+      <c r="A161" s="4"/>
+      <c r="B161" s="3"/>
     </row>
     <row r="162" ht="14.25" customHeight="1">
-      <c r="A162" t="s" s="0">
-        <v>227</v>
-      </c>
-      <c r="B162" s="104" t="s">
-        <v>228</v>
-      </c>
+      <c r="A162" s="4"/>
+      <c r="B162" s="3"/>
     </row>
     <row r="163" ht="14.25" customHeight="1">
       <c r="B163" s="3"/>
@@ -6121,62 +4306,38 @@
       <c r="B171" s="3"/>
     </row>
     <row r="172" ht="14.25" customHeight="1">
-      <c r="A172" t="s" s="0">
-        <v>229</v>
-      </c>
-      <c r="B172" s="105" t="s">
-        <v>191</v>
-      </c>
+      <c r="A172" s="4"/>
+      <c r="B172" s="3"/>
       <c r="E172" s="4"/>
       <c r="F172" s="3"/>
     </row>
     <row r="173" ht="14.25" customHeight="1">
-      <c r="A173" t="s" s="0">
-        <v>230</v>
-      </c>
-      <c r="B173" s="106" t="s">
-        <v>231</v>
-      </c>
+      <c r="A173" s="4"/>
+      <c r="B173" s="3"/>
       <c r="E173" s="4"/>
       <c r="F173" s="3"/>
     </row>
     <row r="174" ht="14.25" customHeight="1">
-      <c r="A174" t="s" s="0">
-        <v>234</v>
-      </c>
-      <c r="B174" s="108" t="s">
-        <v>125</v>
-      </c>
+      <c r="A174" s="4"/>
+      <c r="B174" s="3"/>
       <c r="E174" s="4"/>
       <c r="F174" s="3"/>
     </row>
     <row r="175" ht="14.25" customHeight="1">
-      <c r="A175" t="s" s="0">
-        <v>235</v>
-      </c>
-      <c r="B175" s="109" t="s">
-        <v>236</v>
-      </c>
+      <c r="A175" s="4"/>
+      <c r="B175" s="3"/>
       <c r="E175" s="4"/>
       <c r="F175" s="3"/>
     </row>
     <row r="176" ht="14.25" customHeight="1">
-      <c r="A176" t="s" s="0">
-        <v>237</v>
-      </c>
-      <c r="B176" s="110" t="s">
-        <v>126</v>
-      </c>
+      <c r="A176" s="4"/>
+      <c r="B176" s="3"/>
       <c r="E176" s="4"/>
       <c r="F176" s="3"/>
     </row>
     <row r="177" ht="14.25" customHeight="1">
-      <c r="A177" t="s" s="0">
-        <v>238</v>
-      </c>
-      <c r="B177" s="111" t="s">
-        <v>125</v>
-      </c>
+      <c r="A177" s="4"/>
+      <c r="B177" s="3"/>
       <c r="E177" s="4"/>
       <c r="F177" s="3"/>
     </row>
@@ -6210,122 +4371,74 @@
       <c r="B187" s="3"/>
     </row>
     <row r="188" ht="14.25" customHeight="1">
-      <c r="A188" t="s" s="0">
-        <v>239</v>
-      </c>
-      <c r="B188" s="112" t="s">
-        <v>191</v>
-      </c>
+      <c r="A188" s="4"/>
+      <c r="B188" s="3"/>
       <c r="E188" s="4"/>
       <c r="F188" s="3"/>
     </row>
     <row r="189" ht="14.25" customHeight="1">
-      <c r="A189" t="s" s="0">
-        <v>240</v>
-      </c>
-      <c r="B189" s="113" t="s">
-        <v>241</v>
-      </c>
+      <c r="A189" s="4"/>
+      <c r="B189" s="3"/>
       <c r="E189" s="4"/>
       <c r="F189" s="3"/>
     </row>
     <row r="190" ht="14.25" customHeight="1">
-      <c r="A190" t="s" s="0">
-        <v>242</v>
-      </c>
-      <c r="B190" s="114" t="s">
-        <v>125</v>
-      </c>
+      <c r="A190" s="4"/>
+      <c r="B190" s="3"/>
       <c r="E190" s="4"/>
       <c r="F190" s="3"/>
     </row>
     <row r="191" ht="14.25" customHeight="1">
-      <c r="A191" t="s" s="0">
-        <v>243</v>
-      </c>
-      <c r="B191" s="115" t="s">
-        <v>191</v>
-      </c>
+      <c r="A191" s="4"/>
+      <c r="B191" s="3"/>
       <c r="E191" s="4"/>
       <c r="F191" s="3"/>
     </row>
     <row r="192" ht="14.25" customHeight="1">
-      <c r="A192" t="s" s="0">
-        <v>244</v>
-      </c>
-      <c r="B192" s="116" t="s">
-        <v>245</v>
-      </c>
+      <c r="A192" s="4"/>
+      <c r="B192" s="3"/>
       <c r="E192" s="4"/>
       <c r="F192" s="3"/>
     </row>
     <row r="193" ht="14.25" customHeight="1">
-      <c r="A193" t="s" s="0">
-        <v>246</v>
-      </c>
-      <c r="B193" s="117" t="s">
-        <v>125</v>
-      </c>
+      <c r="A193" s="4"/>
+      <c r="B193" s="3"/>
       <c r="E193" s="4"/>
       <c r="F193" s="3"/>
     </row>
     <row r="194" ht="14.25" customHeight="1">
-      <c r="A194" t="s" s="0">
-        <v>247</v>
-      </c>
-      <c r="B194" s="118" t="s">
-        <v>248</v>
-      </c>
+      <c r="A194" s="4"/>
+      <c r="B194" s="3"/>
       <c r="E194" s="4"/>
       <c r="F194" s="3"/>
     </row>
     <row r="195" ht="14.25" customHeight="1">
-      <c r="A195" t="s" s="0">
-        <v>249</v>
-      </c>
-      <c r="B195" s="119" t="s">
-        <v>125</v>
-      </c>
+      <c r="A195" s="4"/>
+      <c r="B195" s="3"/>
       <c r="E195" s="4"/>
       <c r="F195" s="3"/>
     </row>
     <row r="196" ht="14.25" customHeight="1">
-      <c r="A196" t="s" s="0">
-        <v>250</v>
-      </c>
-      <c r="B196" s="120" t="s">
-        <v>191</v>
-      </c>
+      <c r="A196" s="4"/>
+      <c r="B196" s="3"/>
       <c r="E196" s="4"/>
       <c r="F196" s="3"/>
     </row>
     <row r="197" ht="14.25" customHeight="1">
-      <c r="A197" t="s" s="0">
-        <v>251</v>
-      </c>
-      <c r="B197" s="121" t="s">
-        <v>252</v>
-      </c>
+      <c r="A197" s="4"/>
+      <c r="B197" s="3"/>
       <c r="E197" s="4"/>
       <c r="F197" s="3"/>
     </row>
     <row r="198" ht="14.25" customHeight="1">
-      <c r="A198" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="B198" s="122" t="s">
-        <v>125</v>
-      </c>
+      <c r="A198" s="4"/>
+      <c r="B198" s="3"/>
       <c r="E198" s="4"/>
       <c r="F198" s="3"/>
     </row>
     <row r="199" ht="14.25" customHeight="1">
-      <c r="A199" t="s" s="0">
-        <v>254</v>
-      </c>
-      <c r="B199" s="123" t="s">
-        <v>126</v>
-      </c>
+      <c r="A199" s="4"/>
+      <c r="B199" s="3"/>
       <c r="E199" s="4"/>
       <c r="F199" s="3"/>
     </row>
@@ -7162,12 +5275,8 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="0">
-        <v>104</v>
-      </c>
-      <c r="B1" s="126" t="s">
-        <v>105</v>
-      </c>
+      <c r="A1" s="4"/>
+      <c r="B1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
       <c r="F1" s="3"/>
@@ -7178,12 +5287,8 @@
       <c r="L1" s="3"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="B2" s="127" t="s">
-        <v>29</v>
-      </c>
+      <c r="A2" s="4"/>
+      <c r="B2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="3"/>
@@ -7194,12 +5299,8 @@
       <c r="L2" s="3"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="0">
-        <v>107</v>
-      </c>
-      <c r="B3" s="128" t="s">
-        <v>108</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
       <c r="F3" s="3"/>
@@ -7210,12 +5311,8 @@
       <c r="L3" s="3"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="0">
-        <v>255</v>
-      </c>
-      <c r="B4" s="129" t="s">
-        <v>256</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
       <c r="F4" s="3"/>
@@ -7226,12 +5323,8 @@
       <c r="L4" s="3"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" t="s" s="0">
-        <v>257</v>
-      </c>
-      <c r="B5" s="130" t="s">
-        <v>258</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="4"/>
       <c r="F5" s="3"/>
@@ -7242,12 +5335,8 @@
       <c r="L5" s="3"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" t="s" s="0">
-        <v>102</v>
-      </c>
-      <c r="B6" s="131" t="s">
-        <v>103</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="4"/>
       <c r="F6" s="3"/>
@@ -7258,12 +5347,8 @@
       <c r="L6" s="3"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" t="s" s="0">
-        <v>259</v>
-      </c>
-      <c r="B7" s="132" t="s">
-        <v>260</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
       <c r="F7" s="3"/>
@@ -7274,12 +5359,8 @@
       <c r="L7" s="3"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" t="s" s="0">
-        <v>261</v>
-      </c>
-      <c r="B8" s="133" t="s">
-        <v>262</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
       <c r="F8" s="3"/>
@@ -7290,12 +5371,8 @@
       <c r="L8" s="3"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" t="s" s="0">
-        <v>263</v>
-      </c>
-      <c r="B9" s="134" t="s">
-        <v>125</v>
-      </c>
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
       <c r="F9" s="3"/>
@@ -7306,12 +5383,8 @@
       <c r="L9" s="3"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" t="s" s="0">
-        <v>264</v>
-      </c>
-      <c r="B10" s="135" t="s">
-        <v>265</v>
-      </c>
+      <c r="A10" s="4"/>
+      <c r="B10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
       <c r="F10" s="3"/>
@@ -7322,12 +5395,8 @@
       <c r="L10" s="3"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" t="s" s="0">
-        <v>109</v>
-      </c>
-      <c r="B11" s="136" t="s">
-        <v>110</v>
-      </c>
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="4"/>
       <c r="F11" s="3"/>
@@ -7338,12 +5407,8 @@
       <c r="L11" s="3"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" t="s" s="0">
-        <v>111</v>
-      </c>
-      <c r="B12" s="137" t="s">
-        <v>112</v>
-      </c>
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="4"/>
       <c r="F12" s="3"/>
@@ -7354,12 +5419,8 @@
       <c r="L12" s="3"/>
     </row>
     <row r="13" ht="33.0" customHeight="1">
-      <c r="A13" t="s" s="0">
-        <v>113</v>
-      </c>
-      <c r="B13" s="138" t="s">
-        <v>115</v>
-      </c>
+      <c r="A13" s="4"/>
+      <c r="B13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="4"/>
       <c r="F13" s="3"/>
@@ -7370,12 +5431,8 @@
       <c r="L13" s="3"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" t="s" s="0">
-        <v>266</v>
-      </c>
-      <c r="B14" s="139" t="s">
-        <v>265</v>
-      </c>
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="4"/>
       <c r="F14" s="3"/>
@@ -7386,12 +5443,8 @@
       <c r="L14" s="3"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" t="s" s="0">
-        <v>116</v>
-      </c>
-      <c r="B15" s="140" t="s">
-        <v>117</v>
-      </c>
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="4"/>
       <c r="F15" s="3"/>
@@ -7402,12 +5455,8 @@
       <c r="L15" s="3"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" t="s" s="0">
-        <v>118</v>
-      </c>
-      <c r="B16" s="141" t="s">
-        <v>119</v>
-      </c>
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="4"/>
       <c r="F16" s="3"/>
@@ -7418,12 +5467,8 @@
       <c r="L16" s="3"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" t="s" s="0">
-        <v>120</v>
-      </c>
-      <c r="B17" s="142" t="s">
-        <v>121</v>
-      </c>
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="4"/>
       <c r="F17" s="3"/>
@@ -7434,12 +5479,8 @@
       <c r="L17" s="3"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" t="s" s="0">
-        <v>122</v>
-      </c>
-      <c r="B18" s="143" t="s">
-        <v>123</v>
-      </c>
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="4"/>
       <c r="F18" s="3"/>
@@ -7450,12 +5491,8 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" t="s" s="0">
-        <v>127</v>
-      </c>
-      <c r="B19" s="144" t="s">
-        <v>128</v>
-      </c>
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="4"/>
       <c r="F19" s="3"/>
@@ -7466,12 +5503,8 @@
       <c r="L19" s="3"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" t="s" s="0">
-        <v>129</v>
-      </c>
-      <c r="B20" s="145" t="s">
-        <v>130</v>
-      </c>
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
       <c r="F20" s="3"/>
@@ -7482,12 +5515,8 @@
       <c r="L20" s="3"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" t="s" s="0">
-        <v>131</v>
-      </c>
-      <c r="B21" s="146" t="s">
-        <v>132</v>
-      </c>
+      <c r="A21" s="4"/>
+      <c r="B21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="4"/>
       <c r="F21" s="3"/>
@@ -7498,12 +5527,8 @@
       <c r="L21" s="3"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" t="s" s="0">
-        <v>124</v>
-      </c>
-      <c r="B22" s="147" t="s">
-        <v>125</v>
-      </c>
+      <c r="A22" s="4"/>
+      <c r="B22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="4"/>
       <c r="F22" s="3"/>
@@ -7514,12 +5539,8 @@
       <c r="L22" s="3"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" t="s" s="0">
-        <v>133</v>
-      </c>
-      <c r="B23" s="148" t="s">
-        <v>134</v>
-      </c>
+      <c r="A23" s="4"/>
+      <c r="B23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="4"/>
       <c r="F23" s="3"/>
@@ -7530,12 +5551,8 @@
       <c r="L23" s="3"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" t="s" s="0">
-        <v>129</v>
-      </c>
-      <c r="B24" s="149" t="s">
-        <v>135</v>
-      </c>
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="4"/>
       <c r="F24" s="3"/>
@@ -7546,12 +5563,8 @@
       <c r="L24" s="3"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" t="s" s="0">
-        <v>131</v>
-      </c>
-      <c r="B25" s="150" t="s">
-        <v>136</v>
-      </c>
+      <c r="A25" s="4"/>
+      <c r="B25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="4"/>
       <c r="F25" s="3"/>
@@ -7562,12 +5575,8 @@
       <c r="L25" s="3"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" t="s" s="0">
-        <v>124</v>
-      </c>
-      <c r="B26" s="151" t="s">
-        <v>126</v>
-      </c>
+      <c r="A26" s="4"/>
+      <c r="B26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
       <c r="F26" s="3"/>
@@ -7578,12 +5587,8 @@
       <c r="L26" s="3"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" t="s" s="0">
-        <v>137</v>
-      </c>
-      <c r="B27" s="152" t="s">
-        <v>138</v>
-      </c>
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
       <c r="F27" s="3"/>
@@ -7594,12 +5599,8 @@
       <c r="L27" s="3"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" t="s" s="0">
-        <v>267</v>
-      </c>
-      <c r="B28" s="153" t="s">
-        <v>265</v>
-      </c>
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="4"/>
       <c r="F28" s="3"/>
@@ -7610,12 +5611,8 @@
       <c r="L28" s="3"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" t="s" s="0">
-        <v>139</v>
-      </c>
-      <c r="B29" s="154" t="s">
-        <v>140</v>
-      </c>
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
       <c r="F29" s="3"/>
@@ -7626,12 +5623,8 @@
       <c r="L29" s="3"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" t="s" s="0">
-        <v>141</v>
-      </c>
-      <c r="B30" s="155" t="s">
-        <v>268</v>
-      </c>
+      <c r="A30" s="4"/>
+      <c r="B30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="4"/>
       <c r="F30" s="3"/>
@@ -7642,12 +5635,8 @@
       <c r="L30" s="3"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" t="s" s="0">
-        <v>143</v>
-      </c>
-      <c r="B31" s="156" t="s">
-        <v>126</v>
-      </c>
+      <c r="A31" s="4"/>
+      <c r="B31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
       <c r="F31" s="3"/>
@@ -7658,12 +5647,8 @@
       <c r="L31" s="3"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" t="s" s="0">
-        <v>144</v>
-      </c>
-      <c r="B32" s="157" t="s">
-        <v>125</v>
-      </c>
+      <c r="A32" s="4"/>
+      <c r="B32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="4"/>
       <c r="F32" s="3"/>
@@ -7674,12 +5659,8 @@
       <c r="L32" s="3"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" t="s" s="0">
-        <v>145</v>
-      </c>
-      <c r="B33" s="158" t="s">
-        <v>146</v>
-      </c>
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="4"/>
       <c r="F33" s="3"/>
@@ -7690,12 +5671,8 @@
       <c r="L33" s="3"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" t="s" s="0">
-        <v>269</v>
-      </c>
-      <c r="B34" s="159" t="s">
-        <v>270</v>
-      </c>
+      <c r="A34" s="4"/>
+      <c r="B34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="4"/>
       <c r="F34" s="3"/>
@@ -7706,12 +5683,8 @@
       <c r="L34" s="3"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" t="s" s="0">
-        <v>157</v>
-      </c>
-      <c r="B35" s="160" t="s">
-        <v>271</v>
-      </c>
+      <c r="A35" s="4"/>
+      <c r="B35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="4"/>
       <c r="F35" s="3"/>
@@ -7722,12 +5695,8 @@
       <c r="L35" s="3"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" t="s" s="0">
-        <v>272</v>
-      </c>
-      <c r="B36" s="161" t="s">
-        <v>273</v>
-      </c>
+      <c r="A36" s="4"/>
+      <c r="B36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="4"/>
       <c r="F36" s="3"/>
@@ -7738,12 +5707,8 @@
       <c r="L36" s="3"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" t="s" s="0">
-        <v>147</v>
-      </c>
-      <c r="B37" s="162" t="s">
-        <v>126</v>
-      </c>
+      <c r="A37" s="4"/>
+      <c r="B37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="4"/>
       <c r="F37" s="3"/>
@@ -7754,12 +5719,8 @@
       <c r="L37" s="3"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" t="s" s="0">
-        <v>148</v>
-      </c>
-      <c r="B38" s="163" t="s">
-        <v>125</v>
-      </c>
+      <c r="A38" s="4"/>
+      <c r="B38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="4"/>
       <c r="F38" s="3"/>
@@ -7770,12 +5731,8 @@
       <c r="L38" s="3"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" t="s" s="0">
-        <v>149</v>
-      </c>
-      <c r="B39" s="164" t="s">
-        <v>125</v>
-      </c>
+      <c r="A39" s="4"/>
+      <c r="B39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="4"/>
       <c r="F39" s="3"/>
@@ -7786,12 +5743,8 @@
       <c r="L39" s="3"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" t="s" s="0">
-        <v>150</v>
-      </c>
-      <c r="B40" s="165" t="s">
-        <v>126</v>
-      </c>
+      <c r="A40" s="4"/>
+      <c r="B40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="4"/>
       <c r="F40" s="3"/>
@@ -7802,12 +5755,8 @@
       <c r="L40" s="3"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" t="s" s="0">
-        <v>274</v>
-      </c>
-      <c r="B41" s="166" t="s">
-        <v>152</v>
-      </c>
+      <c r="A41" s="4"/>
+      <c r="B41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="4"/>
       <c r="F41" s="3"/>
@@ -7818,12 +5767,8 @@
       <c r="L41" s="3"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" t="s" s="0">
-        <v>153</v>
-      </c>
-      <c r="B42" s="167" t="s">
-        <v>154</v>
-      </c>
+      <c r="A42" s="4"/>
+      <c r="B42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="4"/>
       <c r="F42" s="3"/>
@@ -7834,12 +5779,8 @@
       <c r="L42" s="3"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" t="s" s="0">
-        <v>155</v>
-      </c>
-      <c r="B43" s="168" t="s">
-        <v>156</v>
-      </c>
+      <c r="A43" s="4"/>
+      <c r="B43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="4"/>
       <c r="F43" s="3"/>
@@ -7850,12 +5791,8 @@
       <c r="L43" s="3"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" t="s" s="0">
-        <v>157</v>
-      </c>
-      <c r="B44" s="169" t="s">
-        <v>275</v>
-      </c>
+      <c r="A44" s="4"/>
+      <c r="B44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="4"/>
       <c r="F44" s="3"/>
@@ -7866,12 +5803,8 @@
       <c r="L44" s="3"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" t="s" s="0">
-        <v>159</v>
-      </c>
-      <c r="B45" s="170" t="s">
-        <v>160</v>
-      </c>
+      <c r="A45" s="4"/>
+      <c r="B45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="4"/>
       <c r="F45" s="3"/>
@@ -7882,12 +5815,8 @@
       <c r="L45" s="3"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" t="s" s="0">
-        <v>276</v>
-      </c>
-      <c r="B46" s="171" t="s">
-        <v>152</v>
-      </c>
+      <c r="A46" s="4"/>
+      <c r="B46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="4"/>
       <c r="F46" s="3"/>
@@ -7896,12 +5825,8 @@
       <c r="L46" s="3"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" t="s" s="0">
-        <v>277</v>
-      </c>
-      <c r="B47" s="172" t="s">
-        <v>100</v>
-      </c>
+      <c r="A47" s="4"/>
+      <c r="B47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="4"/>
       <c r="F47" s="3"/>
@@ -7910,12 +5835,8 @@
       <c r="L47" s="3"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" t="s" s="0">
-        <v>155</v>
-      </c>
-      <c r="B48" s="173" t="s">
-        <v>156</v>
-      </c>
+      <c r="A48" s="4"/>
+      <c r="B48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="4"/>
       <c r="F48" s="3"/>
@@ -7924,12 +5845,8 @@
       <c r="L48" s="3"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" t="s" s="0">
-        <v>157</v>
-      </c>
-      <c r="B49" s="174" t="s">
-        <v>278</v>
-      </c>
+      <c r="A49" s="4"/>
+      <c r="B49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="4"/>
       <c r="F49" s="3"/>
@@ -7938,12 +5855,8 @@
       <c r="L49" s="3"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" t="s" s="0">
-        <v>279</v>
-      </c>
-      <c r="B50" s="175" t="s">
-        <v>280</v>
-      </c>
+      <c r="A50" s="4"/>
+      <c r="B50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="4"/>
       <c r="F50" s="3"/>
@@ -7952,12 +5865,8 @@
       <c r="L50" s="3"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" t="s" s="0">
-        <v>281</v>
-      </c>
-      <c r="B51" s="176" t="s">
-        <v>98</v>
-      </c>
+      <c r="A51" s="4"/>
+      <c r="B51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="4"/>
       <c r="F51" s="3"/>
@@ -7966,12 +5875,8 @@
       <c r="L51" s="3"/>
     </row>
     <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" t="s" s="0">
-        <v>162</v>
-      </c>
-      <c r="B52" s="177" t="s">
-        <v>163</v>
-      </c>
+      <c r="A52" s="4"/>
+      <c r="B52" s="3"/>
       <c r="E52" s="4"/>
       <c r="F52" s="3"/>
       <c r="H52" s="3"/>
@@ -7979,12 +5884,8 @@
       <c r="L52" s="3"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" t="s" s="0">
-        <v>164</v>
-      </c>
-      <c r="B53" s="178" t="s">
-        <v>282</v>
-      </c>
+      <c r="A53" s="4"/>
+      <c r="B53" s="3"/>
       <c r="E53" s="4"/>
       <c r="F53" s="3"/>
       <c r="H53" s="3"/>
@@ -7992,12 +5893,8 @@
       <c r="L53" s="3"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" t="s" s="0">
-        <v>283</v>
-      </c>
-      <c r="B54" s="179" t="s">
-        <v>96</v>
-      </c>
+      <c r="A54" s="4"/>
+      <c r="B54" s="3"/>
       <c r="E54" s="4"/>
       <c r="F54" s="3"/>
       <c r="H54" s="3"/>
@@ -8005,603 +5902,363 @@
       <c r="L54" s="3"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" t="s" s="0">
-        <v>284</v>
-      </c>
-      <c r="B55" s="180" t="s">
-        <v>125</v>
-      </c>
+      <c r="A55" s="4"/>
+      <c r="B55" s="3"/>
       <c r="E55" s="4"/>
       <c r="F55" s="3"/>
       <c r="H55" s="3"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" t="s" s="0">
-        <v>285</v>
-      </c>
-      <c r="B56" s="181" t="s">
-        <v>212</v>
-      </c>
+      <c r="A56" s="4"/>
+      <c r="B56" s="3"/>
       <c r="E56" s="4"/>
       <c r="F56" s="3"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" t="s" s="0">
-        <v>167</v>
-      </c>
-      <c r="B57" s="182" t="s">
-        <v>168</v>
-      </c>
+      <c r="A57" s="4"/>
+      <c r="B57" s="3"/>
       <c r="E57" s="4"/>
       <c r="F57" s="3"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" t="s" s="0">
-        <v>169</v>
-      </c>
-      <c r="B58" s="183" t="s">
-        <v>170</v>
-      </c>
+      <c r="A58" s="4"/>
+      <c r="B58" s="3"/>
       <c r="E58" s="4"/>
       <c r="F58" s="3"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" t="s" s="0">
-        <v>171</v>
-      </c>
-      <c r="B59" s="184" t="s">
-        <v>172</v>
-      </c>
+      <c r="A59" s="4"/>
+      <c r="B59" s="3"/>
       <c r="E59" s="4"/>
       <c r="F59" s="3"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" t="s" s="0">
-        <v>173</v>
-      </c>
-      <c r="B60" s="185" t="s">
-        <v>172</v>
-      </c>
+      <c r="A60" s="4"/>
+      <c r="B60" s="3"/>
       <c r="E60" s="4"/>
       <c r="F60" s="3"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" t="s" s="0">
-        <v>174</v>
-      </c>
-      <c r="B61" s="186" t="s">
-        <v>172</v>
-      </c>
+      <c r="A61" s="4"/>
+      <c r="B61" s="3"/>
       <c r="E61" s="4"/>
       <c r="F61" s="3"/>
     </row>
     <row r="62" ht="14.25" customHeight="1">
-      <c r="A62" t="s" s="0">
-        <v>175</v>
-      </c>
-      <c r="B62" s="187" t="s">
-        <v>172</v>
-      </c>
+      <c r="A62" s="4"/>
+      <c r="B62" s="3"/>
       <c r="E62" s="4"/>
       <c r="F62" s="3"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" t="s" s="0">
-        <v>176</v>
-      </c>
-      <c r="B63" s="188" t="s">
-        <v>172</v>
-      </c>
+      <c r="A63" s="4"/>
+      <c r="B63" s="3"/>
       <c r="E63" s="4"/>
       <c r="F63" s="3"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
-      <c r="A64" t="s" s="0">
-        <v>177</v>
-      </c>
-      <c r="B64" s="189" t="s">
-        <v>180</v>
-      </c>
+      <c r="A64" s="4"/>
+      <c r="B64" s="3"/>
       <c r="E64" s="4"/>
       <c r="F64" s="3"/>
     </row>
     <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" t="s" s="0">
-        <v>179</v>
-      </c>
-      <c r="B65" s="190" t="s">
-        <v>172</v>
-      </c>
+      <c r="A65" s="4"/>
+      <c r="B65" s="3"/>
       <c r="E65" s="4"/>
       <c r="F65" s="3"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
-      <c r="A66" t="s" s="0">
-        <v>181</v>
-      </c>
-      <c r="B66" s="191" t="s">
-        <v>182</v>
-      </c>
+      <c r="A66" s="4"/>
+      <c r="B66" s="3"/>
       <c r="E66" s="4"/>
       <c r="F66" s="3"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" t="s" s="0">
-        <v>183</v>
-      </c>
-      <c r="B67" s="192" t="s">
-        <v>125</v>
-      </c>
+      <c r="A67" s="4"/>
+      <c r="B67" s="3"/>
       <c r="E67" s="4"/>
       <c r="F67" s="3"/>
     </row>
     <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" t="s" s="0">
-        <v>184</v>
-      </c>
-      <c r="B68" s="193" t="s">
-        <v>185</v>
-      </c>
+      <c r="A68" s="4"/>
+      <c r="B68" s="3"/>
       <c r="E68" s="4"/>
       <c r="F68" s="3"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
-      <c r="A69" t="s" s="0">
-        <v>186</v>
-      </c>
-      <c r="B69" s="194" t="s">
-        <v>187</v>
-      </c>
+      <c r="A69" s="4"/>
+      <c r="B69" s="3"/>
       <c r="E69" s="4"/>
       <c r="F69" s="3"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
-      <c r="A70" t="s" s="0">
-        <v>194</v>
-      </c>
-      <c r="B70" s="195" t="s">
-        <v>125</v>
-      </c>
+      <c r="A70" s="4"/>
+      <c r="B70" s="3"/>
       <c r="E70" s="4"/>
       <c r="F70" s="3"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" t="s" s="0">
-        <v>286</v>
-      </c>
-      <c r="B71" s="196" t="s">
-        <v>125</v>
-      </c>
+      <c r="A71" s="4"/>
+      <c r="B71" s="3"/>
       <c r="E71" s="4"/>
       <c r="F71" s="3"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" t="s" s="0">
-        <v>196</v>
-      </c>
-      <c r="B72" s="197" t="s">
-        <v>197</v>
-      </c>
+      <c r="A72" s="4"/>
+      <c r="B72" s="3"/>
       <c r="E72" s="4"/>
       <c r="F72" s="3"/>
     </row>
     <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" t="s" s="0">
-        <v>189</v>
-      </c>
-      <c r="B73" s="198" t="s">
-        <v>125</v>
-      </c>
+      <c r="A73" s="4"/>
+      <c r="B73" s="3"/>
       <c r="E73" s="4"/>
       <c r="F73" s="3"/>
     </row>
     <row r="74" ht="14.25" customHeight="1">
-      <c r="A74" t="s" s="0">
-        <v>287</v>
-      </c>
-      <c r="B74" s="199" t="s">
-        <v>191</v>
-      </c>
+      <c r="A74" s="4"/>
+      <c r="B74" s="3"/>
       <c r="E74" s="4"/>
       <c r="F74" s="3"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
-      <c r="A75" t="s" s="0">
-        <v>192</v>
-      </c>
-      <c r="B75" s="200" t="s">
-        <v>193</v>
-      </c>
+      <c r="A75" s="4"/>
+      <c r="B75" s="3"/>
       <c r="E75" s="4"/>
       <c r="F75" s="3"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" t="s" s="0">
-        <v>288</v>
-      </c>
-      <c r="B76" s="201" t="s">
-        <v>125</v>
-      </c>
+      <c r="A76" s="4"/>
+      <c r="B76" s="3"/>
       <c r="E76" s="4"/>
       <c r="F76" s="3"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
-      <c r="A77" t="s" s="0">
-        <v>289</v>
-      </c>
-      <c r="B77" s="202" t="s">
-        <v>200</v>
-      </c>
+      <c r="A77" s="4"/>
+      <c r="B77" s="3"/>
       <c r="E77" s="4"/>
       <c r="F77" s="3"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
-      <c r="A78" t="s" s="0">
-        <v>201</v>
-      </c>
-      <c r="B78" s="203" t="s">
-        <v>202</v>
-      </c>
+      <c r="A78" s="4"/>
+      <c r="B78" s="3"/>
       <c r="E78" s="4"/>
       <c r="F78" s="3"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
-      <c r="A79" t="s" s="0">
-        <v>203</v>
-      </c>
-      <c r="B79" s="204" t="s">
-        <v>204</v>
-      </c>
+      <c r="A79" s="4"/>
+      <c r="B79" s="3"/>
       <c r="E79" s="4"/>
       <c r="F79" s="3"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" t="s" s="0">
-        <v>205</v>
-      </c>
-      <c r="B80" s="205" t="s">
-        <v>206</v>
-      </c>
+      <c r="A80" s="4"/>
+      <c r="B80" s="3"/>
       <c r="E80" s="4"/>
       <c r="F80" s="3"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" t="s" s="0">
-        <v>207</v>
-      </c>
-      <c r="B81" s="206" t="s">
-        <v>208</v>
-      </c>
+      <c r="A81" s="4"/>
+      <c r="B81" s="3"/>
       <c r="E81" s="4"/>
       <c r="F81" s="3"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" t="s" s="0">
-        <v>209</v>
-      </c>
-      <c r="B82" s="207" t="s">
-        <v>210</v>
-      </c>
+      <c r="A82" s="4"/>
+      <c r="B82" s="3"/>
       <c r="E82" s="4"/>
       <c r="F82" s="3"/>
     </row>
     <row r="83" ht="14.25" customHeight="1">
-      <c r="A83" t="s" s="0">
-        <v>211</v>
-      </c>
-      <c r="B83" s="208" t="s">
-        <v>212</v>
-      </c>
+      <c r="A83" s="4"/>
+      <c r="B83" s="3"/>
       <c r="E83" s="4"/>
       <c r="F83" s="3"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" t="s" s="0">
-        <v>213</v>
-      </c>
-      <c r="B84" s="209" t="s">
-        <v>212</v>
-      </c>
+      <c r="A84" s="4"/>
+      <c r="B84" s="3"/>
       <c r="E84" s="4"/>
       <c r="F84" s="3"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
-      <c r="A85" t="s" s="0">
-        <v>214</v>
-      </c>
-      <c r="B85" s="210" t="s">
-        <v>212</v>
-      </c>
+      <c r="A85" s="4"/>
+      <c r="B85" s="3"/>
       <c r="E85" s="4"/>
       <c r="F85" s="3"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" t="s" s="0">
-        <v>215</v>
-      </c>
-      <c r="B86" s="211" t="s">
-        <v>212</v>
-      </c>
+      <c r="A86" s="4"/>
+      <c r="B86" s="3"/>
       <c r="E86" s="4"/>
       <c r="F86" s="3"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
-      <c r="A87" t="s" s="0">
-        <v>216</v>
-      </c>
-      <c r="B87" s="212" t="s">
-        <v>3</v>
-      </c>
+      <c r="A87" s="4"/>
+      <c r="B87" s="3"/>
       <c r="E87" s="4"/>
       <c r="F87" s="3"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" t="s" s="0">
-        <v>217</v>
-      </c>
-      <c r="B88" s="213" t="s">
-        <v>212</v>
-      </c>
+      <c r="A88" s="4"/>
+      <c r="B88" s="3"/>
       <c r="E88" s="4"/>
       <c r="F88" s="3"/>
     </row>
     <row r="89" ht="14.25" customHeight="1">
-      <c r="A89" t="s" s="0">
-        <v>290</v>
-      </c>
-      <c r="B89" s="214" t="s">
-        <v>212</v>
-      </c>
+      <c r="A89" s="4"/>
+      <c r="B89" s="3"/>
       <c r="E89" s="4"/>
       <c r="F89" s="3"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
-      <c r="A90" t="s" s="0">
-        <v>291</v>
-      </c>
-      <c r="B90" s="215" t="s">
-        <v>125</v>
-      </c>
+      <c r="A90" s="4"/>
+      <c r="B90" s="3"/>
       <c r="E90" s="4"/>
       <c r="F90" s="3"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" t="s" s="0">
-        <v>292</v>
-      </c>
-      <c r="B91" s="216" t="s">
-        <v>191</v>
-      </c>
+      <c r="A91" s="4"/>
+      <c r="B91" s="3"/>
       <c r="E91" s="4"/>
       <c r="F91" s="3"/>
     </row>
     <row r="92" ht="14.25" customHeight="1">
-      <c r="A92" t="s" s="0">
-        <v>221</v>
-      </c>
-      <c r="B92" s="217" t="s">
-        <v>222</v>
-      </c>
+      <c r="A92" s="4"/>
+      <c r="B92" s="3"/>
       <c r="E92" s="4"/>
       <c r="F92" s="3"/>
     </row>
     <row r="93" ht="14.25" customHeight="1">
-      <c r="A93" t="s" s="0">
-        <v>293</v>
-      </c>
-      <c r="B93" s="218" t="s">
-        <v>191</v>
-      </c>
+      <c r="A93" s="4"/>
+      <c r="B93" s="3"/>
       <c r="E93" s="4"/>
       <c r="F93" s="3"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
-      <c r="A94" t="s" s="0">
-        <v>294</v>
-      </c>
-      <c r="B94" s="219" t="s">
-        <v>231</v>
-      </c>
+      <c r="A94" s="4"/>
+      <c r="B94" s="3"/>
       <c r="E94" s="4"/>
       <c r="F94" s="3"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" t="s" s="0">
-        <v>295</v>
-      </c>
-      <c r="B95" s="220" t="s">
-        <v>125</v>
-      </c>
+      <c r="A95" s="4"/>
+      <c r="B95" s="3"/>
       <c r="E95" s="4"/>
       <c r="F95" s="3"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" t="s" s="0">
-        <v>296</v>
-      </c>
-      <c r="B96" s="221" t="s">
-        <v>236</v>
-      </c>
+      <c r="A96" s="4"/>
+      <c r="B96" s="3"/>
       <c r="E96" s="4"/>
       <c r="F96" s="3"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" t="s" s="0">
-        <v>297</v>
-      </c>
-      <c r="B97" s="222" t="s">
-        <v>126</v>
-      </c>
+      <c r="A97" s="4"/>
+      <c r="B97" s="3"/>
       <c r="E97" s="4"/>
       <c r="F97" s="3"/>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" t="s" s="0">
-        <v>298</v>
-      </c>
-      <c r="B98" s="223" t="s">
-        <v>125</v>
-      </c>
+      <c r="A98" s="4"/>
+      <c r="B98" s="3"/>
       <c r="E98" s="4"/>
       <c r="F98" s="3"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
-      <c r="A99" t="s" s="0">
-        <v>299</v>
-      </c>
-      <c r="B99" s="224" t="s">
-        <v>191</v>
-      </c>
+      <c r="A99" s="4"/>
+      <c r="B99" s="3"/>
       <c r="E99" s="4"/>
       <c r="F99" s="3"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
-      <c r="A100" t="s" s="0">
-        <v>240</v>
-      </c>
-      <c r="B100" s="225" t="s">
-        <v>241</v>
-      </c>
+      <c r="A100" s="4"/>
+      <c r="B100" s="3"/>
       <c r="E100" s="4"/>
       <c r="F100" s="3"/>
     </row>
     <row r="101" ht="14.25" customHeight="1">
-      <c r="A101" t="s" s="0">
-        <v>300</v>
-      </c>
-      <c r="B101" s="226" t="s">
-        <v>125</v>
-      </c>
+      <c r="A101" s="4"/>
+      <c r="B101" s="3"/>
       <c r="E101" s="4"/>
       <c r="F101" s="3"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
-      <c r="A102" t="s" s="0">
-        <v>301</v>
-      </c>
-      <c r="B102" s="227" t="s">
-        <v>191</v>
-      </c>
+      <c r="A102" s="4"/>
+      <c r="B102" s="3"/>
       <c r="E102" s="4"/>
       <c r="F102" s="3"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
-      <c r="A103" t="s" s="0">
-        <v>244</v>
-      </c>
-      <c r="B103" s="228" t="s">
-        <v>245</v>
-      </c>
+      <c r="A103" s="4"/>
+      <c r="B103" s="3"/>
       <c r="E103" s="4"/>
       <c r="F103" s="3"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" t="s" s="0">
-        <v>302</v>
-      </c>
-      <c r="B104" s="229" t="s">
-        <v>125</v>
-      </c>
+      <c r="A104" s="4"/>
+      <c r="B104" s="3"/>
       <c r="E104" s="4"/>
       <c r="F104" s="3"/>
     </row>
     <row r="105" ht="14.25" customHeight="1">
-      <c r="A105" t="s" s="0">
-        <v>303</v>
-      </c>
-      <c r="B105" s="230" t="s">
-        <v>191</v>
-      </c>
+      <c r="A105" s="4"/>
+      <c r="B105" s="3"/>
       <c r="E105" s="4"/>
       <c r="F105" s="3"/>
     </row>
     <row r="106" ht="14.25" customHeight="1">
-      <c r="A106" t="s" s="0">
-        <v>251</v>
-      </c>
-      <c r="B106" s="231" t="s">
-        <v>252</v>
-      </c>
+      <c r="A106" s="4"/>
+      <c r="B106" s="3"/>
       <c r="E106" s="4"/>
       <c r="F106" s="3"/>
     </row>
     <row r="107" ht="14.25" customHeight="1">
-      <c r="A107" t="s" s="0">
-        <v>253</v>
-      </c>
-      <c r="B107" s="232" t="s">
-        <v>125</v>
-      </c>
+      <c r="A107" s="4"/>
+      <c r="B107" s="3"/>
       <c r="E107" s="4"/>
       <c r="F107" s="3"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
-      <c r="A108" t="s" s="0">
-        <v>304</v>
-      </c>
-      <c r="B108" s="233" t="s">
-        <v>125</v>
-      </c>
+      <c r="A108" s="4"/>
+      <c r="B108" s="3"/>
       <c r="E108" s="4"/>
       <c r="F108" s="3"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
-      <c r="A109" t="s" s="0">
-        <v>247</v>
-      </c>
-      <c r="B109" s="234" t="s">
-        <v>248</v>
-      </c>
+      <c r="A109" s="4"/>
+      <c r="B109" s="3"/>
       <c r="E109" s="4"/>
       <c r="F109" s="3"/>
     </row>
     <row r="110" ht="14.25" customHeight="1">
-      <c r="A110" t="s" s="0">
-        <v>254</v>
-      </c>
-      <c r="B110" s="235" t="s">
-        <v>126</v>
-      </c>
+      <c r="A110" s="4"/>
+      <c r="B110" s="3"/>
       <c r="E110" s="4"/>
       <c r="F110" s="3"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
-      <c r="A111" t="s" s="0">
-        <v>305</v>
-      </c>
-      <c r="B111" s="236" t="s">
-        <v>224</v>
-      </c>
+      <c r="A111" s="4"/>
+      <c r="B111" s="3"/>
       <c r="E111" s="4"/>
       <c r="F111" s="3"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
-      <c r="A112" t="s" s="0">
-        <v>306</v>
-      </c>
-      <c r="B112" s="237" t="s">
-        <v>226</v>
-      </c>
+      <c r="A112" s="4"/>
+      <c r="B112" s="3"/>
       <c r="E112" s="4"/>
       <c r="F112" s="3"/>
     </row>
     <row r="113" ht="14.25" customHeight="1">
-      <c r="A113" t="s" s="0">
-        <v>227</v>
-      </c>
-      <c r="B113" s="238" t="s">
-        <v>228</v>
-      </c>
+      <c r="A113" s="4"/>
+      <c r="B113" s="3"/>
       <c r="E113" s="4"/>
       <c r="F113" s="3"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
-      <c r="A114" t="s" s="0">
-        <v>188</v>
-      </c>
-      <c r="B114" s="239" t="s">
-        <v>125</v>
-      </c>
+      <c r="A114" s="4"/>
+      <c r="B114" s="3"/>
       <c r="E114" s="4"/>
       <c r="F114" s="3"/>
     </row>

</xml_diff>